<commit_message>
update analysis of results for hydro paper
</commit_message>
<xml_diff>
--- a/hydro/hpc_results/last_results/4months/_latest/4M_NEW_result_comparison.xlsx
+++ b/hydro/hpc_results/last_results/4months/_latest/4M_NEW_result_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\PyPSA\Luca\nodal_zonal_model\hydro\hpc_results\last_results\4months\_latest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9ACA0F-82BB-4C71-ACF7-63E75DBA4361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C6EACA-0534-4D4E-B532-8FED4F9B869B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10935" yWindow="-2475" windowWidth="7080" windowHeight="3675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7080" windowHeight="3672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
   <si>
     <t>f_sum;f_su</t>
   </si>
@@ -109,12 +109,6 @@
   </si>
   <si>
     <t>0;0</t>
-  </si>
-  <si>
-    <t>(35, 'penalty')</t>
-  </si>
-  <si>
-    <t>40;10</t>
   </si>
   <si>
     <t>('zonal_shadow', 'bids')</t>
@@ -149,7 +143,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -193,7 +187,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -485,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O32"/>
+  <dimension ref="B1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,13 +502,13 @@
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>1</v>
@@ -526,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>5</v>
@@ -566,7 +560,7 @@
         <v>17.307823710000001</v>
       </c>
       <c r="J2" s="5">
-        <f>O2/1000</f>
+        <f t="shared" ref="J2:J16" si="0">O2/1000</f>
         <v>41.629046369999998</v>
       </c>
       <c r="K2" s="2">
@@ -590,11 +584,11 @@
         <v>164304000000</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E15" si="0">(D3-$D$2)/1000000</f>
+        <f t="shared" ref="E3:E14" si="1">(D3-$D$2)/1000000</f>
         <v>138</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F15" si="1">(D3-$D$2)/$D$2</f>
+        <f t="shared" ref="F3:F14" si="2">(D3-$D$2)/$D$2</f>
         <v>8.4061255071086582E-4</v>
       </c>
       <c r="G3" s="4">
@@ -607,7 +601,7 @@
         <v>17.177997950000002</v>
       </c>
       <c r="J3" s="5">
-        <f>O3/1000</f>
+        <f t="shared" si="0"/>
         <v>41.629046369999998</v>
       </c>
       <c r="K3" s="2">
@@ -631,11 +625,11 @@
         <v>164325000000</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>159</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.6853185190599758E-4</v>
       </c>
       <c r="G4" s="4">
@@ -648,7 +642,7 @@
         <v>17.28425009</v>
       </c>
       <c r="J4" s="5">
-        <f>O4/1000</f>
+        <f t="shared" si="0"/>
         <v>41.629046369999998</v>
       </c>
       <c r="K4" s="2">
@@ -672,11 +666,11 @@
         <v>165122901662.50101</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>956.90166250100708</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.8288662847423159E-3</v>
       </c>
       <c r="G5" s="4">
@@ -689,7 +683,7 @@
         <v>16.164673727365901</v>
       </c>
       <c r="J5" s="5">
-        <f>O5/1000</f>
+        <f t="shared" si="0"/>
         <v>41.629046370306703</v>
       </c>
       <c r="K5" s="2">
@@ -713,11 +707,11 @@
         <v>164316000000</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1370929425094107E-4</v>
       </c>
       <c r="G6" s="4">
@@ -730,7 +724,7 @@
         <v>17.290399730000001</v>
       </c>
       <c r="J6" s="5">
-        <f>O6/1000</f>
+        <f t="shared" si="0"/>
         <v>41.629046369999998</v>
       </c>
       <c r="K6" s="2">
@@ -754,11 +748,11 @@
         <v>167654000000</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3488</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.1246786788981883E-2</v>
       </c>
       <c r="G7" s="4">
@@ -771,7 +765,7 @@
         <v>17.690126410000001</v>
       </c>
       <c r="J7" s="5">
-        <f>O7/1000</f>
+        <f t="shared" si="0"/>
         <v>60.347176339999997</v>
       </c>
       <c r="K7" s="2">
@@ -795,11 +789,11 @@
         <v>166534000000</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2368</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4424424058574857E-2</v>
       </c>
       <c r="G8" s="4">
@@ -812,7 +806,7 @@
         <v>16.655620089999999</v>
       </c>
       <c r="J8" s="5">
-        <f>O8/1000</f>
+        <f t="shared" si="0"/>
         <v>60.347176339999997</v>
       </c>
       <c r="K8" s="2">
@@ -836,11 +830,11 @@
         <v>164318000000</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>152</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.258920848409537E-4</v>
       </c>
       <c r="G9" s="4">
@@ -853,7 +847,7 @@
         <v>17.085070040000002</v>
       </c>
       <c r="J9" s="5">
-        <f>O9/1000</f>
+        <f t="shared" si="0"/>
         <v>41.629046369999998</v>
       </c>
       <c r="K9" s="2">
@@ -877,11 +871,11 @@
         <v>172999000000</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8833</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.3805294640790417E-2</v>
       </c>
       <c r="G10" s="4">
@@ -894,7 +888,7 @@
         <v>17.676118890000001</v>
       </c>
       <c r="J10" s="5">
-        <f>O10/1000</f>
+        <f t="shared" si="0"/>
         <v>2248.8242740000001</v>
       </c>
       <c r="K10" s="2">
@@ -911,79 +905,79 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
       <c r="D11" s="1">
-        <v>164320000000</v>
+        <v>169876000000</v>
       </c>
       <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>5710</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4781867134485826E-2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>856.59751679999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1.0333478E-2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>17.174239839999998</v>
+      </c>
+      <c r="J11" s="5">
         <f t="shared" si="0"/>
-        <v>154</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" si="1"/>
-        <v>9.3807487543096622E-4</v>
-      </c>
-      <c r="G11" s="4">
-        <v>663.64995090000002</v>
-      </c>
-      <c r="H11" s="3">
-        <v>1.0390213000000001E-2</v>
-      </c>
-      <c r="I11" s="4">
-        <v>17.268534339999999</v>
-      </c>
-      <c r="J11" s="5">
-        <f>O11/1000</f>
-        <v>41.629046369999998</v>
+        <v>2063.6856809999999</v>
       </c>
       <c r="K11" s="2">
-        <v>0</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="L11" s="4">
-        <v>4.3513944440000003</v>
+        <v>1.2672388889999999</v>
       </c>
       <c r="O11" s="5">
-        <v>41629.046369999996</v>
+        <v>2063685.6810000001</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="1">
-        <v>169876000000</v>
+        <v>170209000000</v>
       </c>
       <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>6043</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>3.6810301767722917E-2</v>
+      </c>
+      <c r="G12" s="4">
+        <v>858.72480570000005</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.0373151000000001E-2</v>
+      </c>
+      <c r="I12" s="4">
+        <v>17.240177660000001</v>
+      </c>
+      <c r="J12" s="5">
         <f t="shared" si="0"/>
-        <v>5710</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="1"/>
-        <v>3.4781867134485826E-2</v>
-      </c>
-      <c r="G12" s="4">
-        <v>856.59751679999999</v>
-      </c>
-      <c r="H12" s="3">
-        <v>1.0333478E-2</v>
-      </c>
-      <c r="I12" s="4">
-        <v>17.174239839999998</v>
-      </c>
-      <c r="J12" s="5">
-        <f>O12/1000</f>
-        <v>2063.6856809999999</v>
+        <v>2082.7799530000002</v>
       </c>
       <c r="K12" s="2">
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="L12" s="4">
-        <v>1.2672388889999999</v>
+        <v>1.459430556</v>
       </c>
       <c r="O12" s="5">
-        <v>2063685.6810000001</v>
+        <v>2082779.953</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -991,123 +985,95 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1">
-        <v>170209000000</v>
+        <v>168515000000</v>
       </c>
       <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>4349</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>2.6491478137982288E-2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>849.25833120000004</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1.0253719E-2</v>
+      </c>
+      <c r="I13" s="4">
+        <v>17.041680899999999</v>
+      </c>
+      <c r="J13" s="5">
         <f t="shared" si="0"/>
-        <v>6043</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="1"/>
-        <v>3.6810301767722917E-2</v>
-      </c>
-      <c r="G13" s="4">
-        <v>858.72480570000005</v>
-      </c>
-      <c r="H13" s="3">
-        <v>1.0373151000000001E-2</v>
-      </c>
-      <c r="I13" s="4">
-        <v>17.240177660000001</v>
-      </c>
-      <c r="J13" s="5">
-        <f>O13/1000</f>
-        <v>2082.7799530000002</v>
+        <v>1853.636483</v>
       </c>
       <c r="K13" s="2">
-        <v>2.0999999999999999E-3</v>
+        <v>1.9E-3</v>
       </c>
       <c r="L13" s="4">
-        <v>1.459430556</v>
+        <v>1.199325</v>
       </c>
       <c r="O13" s="5">
-        <v>2082779.953</v>
+        <v>1853636.483</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1">
-        <v>168515000000</v>
+        <v>170089000000</v>
       </c>
       <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>5923</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>3.607933433232216E-2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>859.3487288</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.0321349E-2</v>
+      </c>
+      <c r="I14" s="4">
+        <v>17.154082679999998</v>
+      </c>
+      <c r="J14" s="5">
         <f t="shared" si="0"/>
-        <v>4349</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="1"/>
-        <v>2.6491478137982288E-2</v>
-      </c>
-      <c r="G14" s="4">
-        <v>849.25833120000004</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1.0253719E-2</v>
-      </c>
-      <c r="I14" s="4">
-        <v>17.041680899999999</v>
-      </c>
-      <c r="J14" s="5">
-        <f>O14/1000</f>
-        <v>1853.636483</v>
+        <v>2181.2939380000003</v>
       </c>
       <c r="K14" s="2">
-        <v>1.9E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="L14" s="4">
-        <v>1.199325</v>
+        <v>1.3818527780000001</v>
       </c>
       <c r="O14" s="5">
-        <v>1853636.483</v>
+        <v>2181293.9380000001</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="1">
-        <v>170089000000</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="F15" s="1"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5">
         <f t="shared" si="0"/>
-        <v>5923</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="1"/>
-        <v>3.607933433232216E-2</v>
-      </c>
-      <c r="G15" s="4">
-        <v>859.3487288</v>
-      </c>
-      <c r="H15" s="3">
-        <v>1.0321349E-2</v>
-      </c>
-      <c r="I15" s="4">
-        <v>17.154082679999998</v>
-      </c>
-      <c r="J15" s="5">
-        <f>O15/1000</f>
-        <v>2181.2939380000003</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="L15" s="4">
-        <v>1.3818527780000001</v>
-      </c>
-      <c r="O15" s="5">
-        <v>2181293.9380000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="4"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F16" s="1"/>
@@ -1115,630 +1081,576 @@
       <c r="H16" s="3"/>
       <c r="I16" s="4"/>
       <c r="J16" s="5">
-        <f>O16/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="4"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F17" s="1"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="5">
-        <f>O17/1000</f>
+    <row r="17" spans="2:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="4"/>
+      <c r="D17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="2:15" ht="72" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>0.5</v>
-      </c>
-      <c r="C18" s="6" t="s">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>164338806849.48801</v>
+      </c>
+      <c r="E18" s="5">
+        <f>(D18-$D$18)/1000000</f>
         <v>0</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="O18" s="5"/>
+      <c r="F18" s="3">
+        <f>(D18-$D$18)/$D$18</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>763.30115822094604</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2.9286032322001401E-2</v>
+      </c>
+      <c r="I18" s="4">
+        <v>48.673385719166298</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" ref="J18:J30" si="3">O18/1000</f>
+        <v>452.94886011163601</v>
+      </c>
+      <c r="K18" s="3">
+        <v>4.5628115885961698E-4</v>
+      </c>
+      <c r="L18" s="4">
+        <v>203.199930555555</v>
+      </c>
+      <c r="O18" s="5">
+        <v>452948.86011163599</v>
+      </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>164338806849.48801</v>
+        <v>164503100017.349</v>
       </c>
       <c r="E19" s="5">
-        <f>(D19-$D$19)/1000000</f>
-        <v>0</v>
+        <f t="shared" ref="E19:E30" si="4">(D19-$D$18)/1000000</f>
+        <v>164.29316786099244</v>
       </c>
       <c r="F19" s="3">
-        <f>(D19-$D$19)/$D$19</f>
-        <v>0</v>
+        <f t="shared" ref="F19:F30" si="5">(D19-$D$18)/$D$18</f>
+        <v>9.997222872103642E-4</v>
       </c>
       <c r="G19" s="4">
-        <v>763.30115822094604</v>
+        <v>763.30272833587901</v>
       </c>
       <c r="H19" s="3">
-        <v>2.9286032322001401E-2</v>
+        <v>2.8891555734258799E-2</v>
       </c>
       <c r="I19" s="4">
-        <v>48.673385719166298</v>
+        <v>48.017765630338197</v>
       </c>
       <c r="J19" s="5">
-        <f>O19/1000</f>
-        <v>452.94886011163601</v>
+        <f t="shared" si="3"/>
+        <v>452.87796894704803</v>
       </c>
       <c r="K19" s="3">
-        <v>4.5628115885961698E-4</v>
+        <v>4.56209746155933E-4</v>
       </c>
       <c r="L19" s="4">
-        <v>203.199930555555</v>
+        <v>17.801352777777701</v>
       </c>
       <c r="O19" s="5">
-        <v>452948.86011163599</v>
+        <v>452877.96894704801</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D20">
-        <v>164503100017.349</v>
+        <v>164432023348.556</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" ref="E20:E32" si="2">(D20-$D$19)/1000000</f>
-        <v>164.29316786099244</v>
+        <f t="shared" si="4"/>
+        <v>93.216499067993169</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" ref="F20:F32" si="3">(D20-$D$19)/$D$19</f>
-        <v>9.997222872103642E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.6722146676753469E-4</v>
       </c>
       <c r="G20" s="4">
-        <v>763.30272833587901</v>
+        <v>763.30324310749904</v>
       </c>
       <c r="H20" s="3">
-        <v>2.8891555734258799E-2</v>
+        <v>2.9002971216570701E-2</v>
       </c>
       <c r="I20" s="4">
-        <v>48.017765630338197</v>
+        <v>48.202938161940502</v>
       </c>
       <c r="J20" s="5">
-        <f>O20/1000</f>
-        <v>452.87796894704803</v>
+        <f t="shared" si="3"/>
+        <v>452.87813375543902</v>
       </c>
       <c r="K20" s="3">
-        <v>4.56209746155933E-4</v>
+        <v>4.5620991217680198E-4</v>
       </c>
       <c r="L20" s="4">
-        <v>17.801352777777701</v>
+        <v>8.9953305555555492</v>
       </c>
       <c r="O20" s="5">
-        <v>452877.96894704801</v>
+        <v>452878.13375543902</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>164432023348.556</v>
+        <v>165560826958.164</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="2"/>
-        <v>93.216499067993169</v>
+        <f t="shared" si="4"/>
+        <v>1222.0201086759948</v>
       </c>
       <c r="F21" s="3">
+        <f t="shared" si="5"/>
+        <v>7.4359801686719011E-3</v>
+      </c>
+      <c r="G21" s="4">
+        <v>755.26506320152305</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2.8875110644618701E-2</v>
+      </c>
+      <c r="I21" s="4">
+        <v>47.990433891356297</v>
+      </c>
+      <c r="J21" s="5">
         <f t="shared" si="3"/>
-        <v>5.6722146676753469E-4</v>
-      </c>
-      <c r="G21" s="4">
-        <v>763.30324310749904</v>
-      </c>
-      <c r="H21" s="3">
-        <v>2.9002971216570701E-2</v>
-      </c>
-      <c r="I21" s="4">
-        <v>48.202938161940502</v>
-      </c>
-      <c r="J21" s="5">
-        <f>O21/1000</f>
-        <v>452.87813375543902</v>
-      </c>
-      <c r="K21" s="3">
-        <v>4.5620991217680198E-4</v>
+        <v>430.81821513039603</v>
+      </c>
+      <c r="K21" s="2">
+        <v>4.3398770097154003E-4</v>
       </c>
       <c r="L21" s="4">
-        <v>8.9953305555555492</v>
+        <v>38.563319444444403</v>
       </c>
       <c r="O21" s="5">
-        <v>452878.13375543902</v>
+        <v>430818.21513039601</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22">
-        <v>165560826958.164</v>
+        <v>164497869022.21701</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="2"/>
-        <v>1222.0201086759948</v>
+        <f t="shared" si="4"/>
+        <v>159.06217272900392</v>
       </c>
       <c r="F22" s="3">
+        <f t="shared" si="5"/>
+        <v>9.6789173402410801E-4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>763.303347437463</v>
+      </c>
+      <c r="H22" s="3">
+        <v>2.9109042044749501E-2</v>
+      </c>
+      <c r="I22" s="4">
+        <v>48.379227878373698</v>
+      </c>
+      <c r="J22" s="5">
         <f t="shared" si="3"/>
-        <v>7.4359801686719011E-3</v>
-      </c>
-      <c r="G22" s="4">
-        <v>755.26506320152305</v>
-      </c>
-      <c r="H22" s="3">
-        <v>2.8875110644618701E-2</v>
-      </c>
-      <c r="I22" s="4">
-        <v>47.990433891356297</v>
-      </c>
-      <c r="J22" s="5">
-        <f>O22/1000</f>
-        <v>430.81821513039603</v>
-      </c>
-      <c r="K22" s="2">
-        <v>4.3398770097154003E-4</v>
+        <v>452.87796894704803</v>
+      </c>
+      <c r="K22" s="3">
+        <v>4.56209746155933E-4</v>
       </c>
       <c r="L22" s="4">
-        <v>38.563319444444403</v>
+        <v>18.4451583333333</v>
       </c>
       <c r="O22" s="5">
-        <v>430818.21513039601</v>
+        <v>452877.96894704801</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D23">
-        <v>164497869022.21701</v>
+        <v>168144940704.85001</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="2"/>
-        <v>159.06217272900392</v>
+        <f t="shared" si="4"/>
+        <v>3806.1338553619994</v>
       </c>
       <c r="F23" s="3">
+        <f t="shared" si="5"/>
+        <v>2.3160286534439186E-2</v>
+      </c>
+      <c r="G23" s="4">
+        <v>757.93408866060201</v>
+      </c>
+      <c r="H23" s="3">
+        <v>2.94478108913361E-2</v>
+      </c>
+      <c r="I23" s="4">
+        <v>48.942261701400703</v>
+      </c>
+      <c r="J23" s="5">
         <f t="shared" si="3"/>
-        <v>9.6789173402410801E-4</v>
-      </c>
-      <c r="G23" s="4">
-        <v>763.303347437463</v>
-      </c>
-      <c r="H23" s="3">
-        <v>2.9109042044749501E-2</v>
-      </c>
-      <c r="I23" s="4">
-        <v>48.379227878373698</v>
-      </c>
-      <c r="J23" s="5">
-        <f>O23/1000</f>
-        <v>452.87796894704803</v>
+        <v>494.82874138386097</v>
       </c>
       <c r="K23" s="3">
-        <v>4.56209746155933E-4</v>
+        <v>4.9846914616371197E-4</v>
       </c>
       <c r="L23" s="4">
-        <v>18.4451583333333</v>
+        <v>5.4399638888888804</v>
       </c>
       <c r="O23" s="5">
-        <v>452877.96894704801</v>
+        <v>494828.74138386099</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D24">
-        <v>168144940704.85001</v>
+        <v>167766254246.29599</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="2"/>
-        <v>3806.1338553619994</v>
+        <f t="shared" si="4"/>
+        <v>3427.4473968079833</v>
       </c>
       <c r="F24" s="3">
+        <f t="shared" si="5"/>
+        <v>2.0855983212456075E-2</v>
+      </c>
+      <c r="G24" s="4">
+        <v>779.31802085494598</v>
+      </c>
+      <c r="H24" s="3">
+        <v>2.9225391053953401E-2</v>
+      </c>
+      <c r="I24" s="4">
+        <v>48.572599931670602</v>
+      </c>
+      <c r="J24" s="5">
         <f t="shared" si="3"/>
-        <v>2.3160286534439186E-2</v>
-      </c>
-      <c r="G24" s="4">
-        <v>757.93408866060201</v>
-      </c>
-      <c r="H24" s="3">
-        <v>2.94478108913361E-2</v>
-      </c>
-      <c r="I24" s="4">
-        <v>48.942261701400703</v>
-      </c>
-      <c r="J24" s="5">
-        <f>O24/1000</f>
-        <v>494.82874138386097</v>
+        <v>551.57213241256704</v>
       </c>
       <c r="K24" s="3">
-        <v>4.9846914616371197E-4</v>
+        <v>5.5562999255555703E-4</v>
       </c>
       <c r="L24" s="4">
-        <v>5.4399638888888804</v>
+        <v>2.0646527777777699</v>
       </c>
       <c r="O24" s="5">
-        <v>494828.74138386099</v>
+        <v>551572.13241256704</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D25">
-        <v>167766254246.29599</v>
+        <v>164499124098.638</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="2"/>
-        <v>3427.4473968079833</v>
+        <f t="shared" si="4"/>
+        <v>160.3172491499939</v>
       </c>
       <c r="F25" s="3">
+        <f t="shared" si="5"/>
+        <v>9.7552886152339345E-4</v>
+      </c>
+      <c r="G25" s="4">
+        <v>763.30317094849897</v>
+      </c>
+      <c r="H25" s="3">
+        <v>2.9041000486363499E-2</v>
+      </c>
+      <c r="I25" s="4">
+        <v>48.266142808336099</v>
+      </c>
+      <c r="J25" s="5">
         <f t="shared" si="3"/>
-        <v>2.0855983212456075E-2</v>
-      </c>
-      <c r="G25" s="4">
-        <v>779.31802085494598</v>
-      </c>
-      <c r="H25" s="3">
-        <v>2.9225391053953401E-2</v>
-      </c>
-      <c r="I25" s="4">
-        <v>48.572599931670602</v>
-      </c>
-      <c r="J25" s="5">
-        <f>O25/1000</f>
-        <v>551.57213241256704</v>
+        <v>452.87796894704803</v>
       </c>
       <c r="K25" s="3">
-        <v>5.5562999255555703E-4</v>
+        <v>4.56209746155933E-4</v>
       </c>
       <c r="L25" s="4">
-        <v>2.0646527777777699</v>
+        <v>17.440630555555501</v>
       </c>
       <c r="O25" s="5">
-        <v>551572.13241256704</v>
+        <v>452877.96894704801</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D26">
-        <v>164499124098.638</v>
+        <v>172749103564.10101</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="2"/>
-        <v>160.3172491499939</v>
+        <f t="shared" si="4"/>
+        <v>8410.2967146130068</v>
       </c>
       <c r="F26" s="3">
+        <f t="shared" si="5"/>
+        <v>5.1176571595263523E-2</v>
+      </c>
+      <c r="G26" s="4">
+        <v>902.74109126400003</v>
+      </c>
+      <c r="H26" s="3">
+        <v>2.9776712684138701E-2</v>
+      </c>
+      <c r="I26" s="4">
+        <v>49.488896481038601</v>
+      </c>
+      <c r="J26" s="5">
         <f t="shared" si="3"/>
-        <v>9.7552886152339345E-4</v>
-      </c>
-      <c r="G26" s="4">
-        <v>763.30317094849897</v>
-      </c>
-      <c r="H26" s="3">
-        <v>2.9041000486363499E-2</v>
-      </c>
-      <c r="I26" s="4">
-        <v>48.266142808336099</v>
-      </c>
-      <c r="J26" s="5">
-        <f>O26/1000</f>
-        <v>452.87796894704803</v>
+        <v>2383.6464164020999</v>
       </c>
       <c r="K26" s="3">
-        <v>4.56209746155933E-4</v>
+        <v>2.40118266092879E-3</v>
       </c>
       <c r="L26" s="4">
-        <v>17.440630555555501</v>
+        <v>1.2883749999999901</v>
       </c>
       <c r="O26" s="5">
-        <v>452877.96894704801</v>
+        <v>2383646.4164021001</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D27">
-        <v>172749103564.10101</v>
+        <v>169765206224.92099</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" si="2"/>
-        <v>8410.2967146130068</v>
+        <f t="shared" si="4"/>
+        <v>5426.3993754329831</v>
       </c>
       <c r="F27" s="3">
+        <f t="shared" si="5"/>
+        <v>3.3019586057983413E-2</v>
+      </c>
+      <c r="G27" s="4">
+        <v>902.37783980032202</v>
+      </c>
+      <c r="H27" s="3">
+        <v>2.9066695938926201E-2</v>
+      </c>
+      <c r="I27" s="4">
+        <v>48.3088486504953</v>
+      </c>
+      <c r="J27" s="5">
         <f t="shared" si="3"/>
-        <v>5.1176571595263523E-2</v>
-      </c>
-      <c r="G27" s="4">
-        <v>902.74109126400003</v>
-      </c>
-      <c r="H27" s="3">
-        <v>2.9776712684138701E-2</v>
-      </c>
-      <c r="I27" s="4">
-        <v>49.488896481038601</v>
-      </c>
-      <c r="J27" s="5">
-        <f>O27/1000</f>
-        <v>2383.6464164020999</v>
+        <v>2392.9401193334602</v>
       </c>
       <c r="K27" s="3">
-        <v>2.40118266092879E-3</v>
+        <v>2.4105447366884599E-3</v>
       </c>
       <c r="L27" s="4">
-        <v>1.2883749999999901</v>
+        <v>1.3506722222222201</v>
       </c>
       <c r="O27" s="5">
-        <v>2383646.4164021001</v>
+        <v>2392940.11933346</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D28">
-        <v>164488958761.39301</v>
+        <v>169574366598.38501</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="2"/>
-        <v>150.15191190499877</v>
+        <f t="shared" si="4"/>
+        <v>5235.5597488970034</v>
       </c>
       <c r="F28" s="3">
+        <f t="shared" si="5"/>
+        <v>3.1858328834601213E-2</v>
+      </c>
+      <c r="G28" s="4">
+        <v>904.69358503410194</v>
+      </c>
+      <c r="H28" s="3">
+        <v>2.8766778616614301E-2</v>
+      </c>
+      <c r="I28" s="4">
+        <v>47.810386060813101</v>
+      </c>
+      <c r="J28" s="5">
         <f t="shared" si="3"/>
-        <v>9.1367288581155088E-4</v>
-      </c>
-      <c r="G28" s="4">
-        <v>758.44992226039506</v>
-      </c>
-      <c r="H28" s="3">
-        <v>2.9078618628915299E-2</v>
-      </c>
-      <c r="I28" s="4">
-        <v>48.328664161257201</v>
-      </c>
-      <c r="J28" s="5">
-        <f>O28/1000</f>
-        <v>457.58881637771202</v>
+        <v>2486.5863975710599</v>
       </c>
       <c r="K28" s="3">
-        <v>4.60955250812562E-4</v>
+        <v>2.5048799610813701E-3</v>
       </c>
       <c r="L28" s="4">
-        <v>7.85828333333333</v>
+        <v>1.2868305555555499</v>
       </c>
       <c r="O28" s="5">
-        <v>457588.81637771201</v>
+        <v>2486586.3975710599</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
         <v>27</v>
       </c>
       <c r="D29">
-        <v>169765206224.92099</v>
+        <v>170133834072.98199</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="2"/>
-        <v>5426.3993754329831</v>
+        <f t="shared" si="4"/>
+        <v>5795.0272234939885</v>
       </c>
       <c r="F29" s="3">
+        <f t="shared" si="5"/>
+        <v>3.5262682835475644E-2</v>
+      </c>
+      <c r="G29" s="4">
+        <v>902.18882150765398</v>
+      </c>
+      <c r="H29" s="3">
+        <v>2.9043261686188999E-2</v>
+      </c>
+      <c r="I29" s="4">
+        <v>48.269900922446098</v>
+      </c>
+      <c r="J29" s="5">
         <f t="shared" si="3"/>
-        <v>3.3019586057983413E-2</v>
-      </c>
-      <c r="G29" s="4">
-        <v>902.37783980032202</v>
-      </c>
-      <c r="H29" s="3">
-        <v>2.9066695938926201E-2</v>
-      </c>
-      <c r="I29" s="4">
-        <v>48.3088486504953</v>
-      </c>
-      <c r="J29" s="5">
-        <f>O29/1000</f>
-        <v>2392.9401193334602</v>
+        <v>2375.8689505427801</v>
       </c>
       <c r="K29" s="3">
-        <v>2.4105447366884599E-3</v>
+        <v>2.3933479770432702E-3</v>
       </c>
       <c r="L29" s="4">
-        <v>1.3506722222222201</v>
+        <v>2.3260888888888802</v>
       </c>
       <c r="O29" s="5">
-        <v>2392940.11933346</v>
+        <v>2375868.9505427801</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D30">
-        <v>169574366598.38501</v>
+        <v>170239833934.20801</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="2"/>
-        <v>5235.5597488970034</v>
+        <f t="shared" si="4"/>
+        <v>5901.0270847200009</v>
       </c>
       <c r="F30" s="3">
+        <f t="shared" si="5"/>
+        <v>3.5907690933429617E-2</v>
+      </c>
+      <c r="G30" s="4">
+        <v>902.44249564082395</v>
+      </c>
+      <c r="H30" s="3">
+        <v>2.8995982053473601E-2</v>
+      </c>
+      <c r="I30" s="4">
+        <v>48.1913221728732</v>
+      </c>
+      <c r="J30" s="5">
         <f t="shared" si="3"/>
-        <v>3.1858328834601213E-2</v>
-      </c>
-      <c r="G30" s="4">
-        <v>904.69358503410194</v>
-      </c>
-      <c r="H30" s="3">
-        <v>2.8766778616614301E-2</v>
-      </c>
-      <c r="I30" s="4">
-        <v>47.810386060813101</v>
-      </c>
-      <c r="J30" s="5">
-        <f>O30/1000</f>
-        <v>2486.5863975710599</v>
+        <v>2397.7714098577003</v>
       </c>
       <c r="K30" s="3">
-        <v>2.5048799610813701E-3</v>
+        <v>2.41541157052627E-3</v>
       </c>
       <c r="L30" s="4">
-        <v>1.2868305555555499</v>
+        <v>1.28118611111111</v>
       </c>
       <c r="O30" s="5">
-        <v>2486586.3975710599</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31">
-        <v>170133834072.98199</v>
-      </c>
-      <c r="E31" s="5">
-        <f t="shared" si="2"/>
-        <v>5795.0272234939885</v>
-      </c>
-      <c r="F31" s="3">
-        <f t="shared" si="3"/>
-        <v>3.5262682835475644E-2</v>
-      </c>
-      <c r="G31" s="4">
-        <v>902.18882150765398</v>
-      </c>
-      <c r="H31" s="3">
-        <v>2.9043261686188999E-2</v>
-      </c>
-      <c r="I31" s="4">
-        <v>48.269900922446098</v>
-      </c>
-      <c r="J31" s="5">
-        <f>O31/1000</f>
-        <v>2375.8689505427801</v>
-      </c>
-      <c r="K31" s="3">
-        <v>2.3933479770432702E-3</v>
-      </c>
-      <c r="L31" s="4">
-        <v>2.3260888888888802</v>
-      </c>
-      <c r="O31" s="5">
-        <v>2375868.9505427801</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32">
-        <v>170239833934.20801</v>
-      </c>
-      <c r="E32" s="5">
-        <f t="shared" si="2"/>
-        <v>5901.0270847200009</v>
-      </c>
-      <c r="F32" s="3">
-        <f t="shared" si="3"/>
-        <v>3.5907690933429617E-2</v>
-      </c>
-      <c r="G32" s="4">
-        <v>902.44249564082395</v>
-      </c>
-      <c r="H32" s="3">
-        <v>2.8995982053473601E-2</v>
-      </c>
-      <c r="I32" s="4">
-        <v>48.1913221728732</v>
-      </c>
-      <c r="J32" s="5">
-        <f>O32/1000</f>
-        <v>2397.7714098577003</v>
-      </c>
-      <c r="K32" s="3">
-        <v>2.41541157052627E-3</v>
-      </c>
-      <c r="L32" s="4">
-        <v>1.28118611111111</v>
-      </c>
-      <c r="O32" s="5">
         <v>2397771.4098577001</v>
       </c>
     </row>

</xml_diff>